<commit_message>
comfirmar cambios de ramdon
</commit_message>
<xml_diff>
--- a/resultados_parametros_random_search.xlsx
+++ b/resultados_parametros_random_search.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1962,10 +1962,8 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>04</t>
-        </is>
+      <c r="A52" t="n">
+        <v>4</v>
       </c>
       <c r="B52" t="n">
         <v>0.03901611516873042</v>
@@ -1996,10 +1994,8 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>41</t>
-        </is>
+      <c r="A53" t="n">
+        <v>41</v>
       </c>
       <c r="B53" t="n">
         <v>0.03837998335560163</v>
@@ -2030,10 +2026,8 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="A54" t="n">
+        <v>11</v>
       </c>
       <c r="B54" t="n">
         <v>0.03795589506626129</v>
@@ -2064,10 +2058,8 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+      <c r="A55" t="n">
+        <v>35</v>
       </c>
       <c r="B55" t="n">
         <v>0.03774385154247284</v>
@@ -2098,10 +2090,8 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="A56" t="n">
+        <v>16</v>
       </c>
       <c r="B56" t="n">
         <v>0.03753180553515752</v>
@@ -2132,173 +2122,503 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
+      <c r="A57" t="n">
+        <v>3</v>
+      </c>
+      <c r="B57" t="n">
+        <v>0.03710771972934405</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F57" t="n">
+        <v>320</v>
+      </c>
+      <c r="G57" t="n">
+        <v>256</v>
+      </c>
+      <c r="H57" t="n">
+        <v>64</v>
+      </c>
+      <c r="I57" t="n">
+        <v>100</v>
+      </c>
+      <c r="J57" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>42</v>
+      </c>
+      <c r="B58" t="n">
+        <v>0.03710771848758062</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F58" t="n">
+        <v>416</v>
+      </c>
+      <c r="G58" t="n">
+        <v>192</v>
+      </c>
+      <c r="H58" t="n">
+        <v>128</v>
+      </c>
+      <c r="I58" t="n">
+        <v>100</v>
+      </c>
+      <c r="J58" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>5</v>
+      </c>
+      <c r="B59" t="n">
+        <v>0.03689567372202873</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F59" t="n">
+        <v>256</v>
+      </c>
+      <c r="G59" t="n">
+        <v>160</v>
+      </c>
+      <c r="H59" t="n">
+        <v>96</v>
+      </c>
+      <c r="I59" t="n">
+        <v>100</v>
+      </c>
+      <c r="J59" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>23</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0.03647158667445183</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F60" t="n">
+        <v>512</v>
+      </c>
+      <c r="G60" t="n">
+        <v>224</v>
+      </c>
+      <c r="H60" t="n">
+        <v>96</v>
+      </c>
+      <c r="I60" t="n">
+        <v>100</v>
+      </c>
+      <c r="J60" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>21</v>
+      </c>
+      <c r="B61" t="n">
+        <v>0.03625954315066338</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F61" t="n">
+        <v>256</v>
+      </c>
+      <c r="G61" t="n">
+        <v>128</v>
+      </c>
+      <c r="H61" t="n">
+        <v>96</v>
+      </c>
+      <c r="I61" t="n">
+        <v>100</v>
+      </c>
+      <c r="J61" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>0.03795589506626129</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F62" t="n">
+        <v>416</v>
+      </c>
+      <c r="G62" t="n">
+        <v>192</v>
+      </c>
+      <c r="H62" t="n">
+        <v>128</v>
+      </c>
+      <c r="I62" t="n">
+        <v>100</v>
+      </c>
+      <c r="J62" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>0.03774385154247284</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F63" t="n">
+        <v>384</v>
+      </c>
+      <c r="G63" t="n">
+        <v>256</v>
+      </c>
+      <c r="H63" t="n">
+        <v>128</v>
+      </c>
+      <c r="I63" t="n">
+        <v>100</v>
+      </c>
+      <c r="J63" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>0.03774385154247284</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F64" t="n">
+        <v>416</v>
+      </c>
+      <c r="G64" t="n">
+        <v>224</v>
+      </c>
+      <c r="H64" t="n">
+        <v>128</v>
+      </c>
+      <c r="I64" t="n">
+        <v>100</v>
+      </c>
+      <c r="J64" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>0.03710771848758062</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F65" t="n">
+        <v>480</v>
+      </c>
+      <c r="G65" t="n">
+        <v>256</v>
+      </c>
+      <c r="H65" t="n">
+        <v>96</v>
+      </c>
+      <c r="I65" t="n">
+        <v>100</v>
+      </c>
+      <c r="J65" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0.03710771848758062</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F66" t="n">
+        <v>512</v>
+      </c>
+      <c r="G66" t="n">
+        <v>192</v>
+      </c>
+      <c r="H66" t="n">
+        <v>64</v>
+      </c>
+      <c r="I66" t="n">
+        <v>100</v>
+      </c>
+      <c r="J66" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0.03689567496379217</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F67" t="n">
+        <v>256</v>
+      </c>
+      <c r="G67" t="n">
+        <v>224</v>
+      </c>
+      <c r="H67" t="n">
+        <v>64</v>
+      </c>
+      <c r="I67" t="n">
+        <v>100</v>
+      </c>
+      <c r="J67" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>0.03689567496379217</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F68" t="n">
+        <v>480</v>
+      </c>
+      <c r="G68" t="n">
+        <v>256</v>
+      </c>
+      <c r="H68" t="n">
+        <v>128</v>
+      </c>
+      <c r="I68" t="n">
+        <v>100</v>
+      </c>
+      <c r="J68" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>0.03668362895647685</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F69" t="n">
+        <v>384</v>
+      </c>
+      <c r="G69" t="n">
+        <v>224</v>
+      </c>
+      <c r="H69" t="n">
+        <v>96</v>
+      </c>
+      <c r="I69" t="n">
+        <v>100</v>
+      </c>
+      <c r="J69" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
         <is>
           <t>03</t>
         </is>
       </c>
-      <c r="B57" t="n">
-        <v>0.03710771972934405</v>
-      </c>
-      <c r="C57" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="D57" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E57" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="F57" t="n">
-        <v>320</v>
-      </c>
-      <c r="G57" t="n">
-        <v>256</v>
-      </c>
-      <c r="H57" t="n">
-        <v>64</v>
-      </c>
-      <c r="I57" t="n">
-        <v>100</v>
-      </c>
-      <c r="J57" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
+      <c r="B70" t="n">
+        <v>0.03647158667445183</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F70" t="n">
+        <v>512</v>
+      </c>
+      <c r="G70" t="n">
+        <v>128</v>
+      </c>
+      <c r="H70" t="n">
+        <v>96</v>
+      </c>
+      <c r="I70" t="n">
+        <v>100</v>
+      </c>
+      <c r="J70" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>27</t>
         </is>
       </c>
-      <c r="B58" t="n">
-        <v>0.03710771848758062</v>
-      </c>
-      <c r="C58" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="D58" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="E58" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="F58" t="n">
-        <v>416</v>
-      </c>
-      <c r="G58" t="n">
+      <c r="B71" t="n">
+        <v>0.03583545486132304</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F71" t="n">
+        <v>384</v>
+      </c>
+      <c r="G71" t="n">
         <v>192</v>
       </c>
-      <c r="H58" t="n">
-        <v>128</v>
-      </c>
-      <c r="I58" t="n">
-        <v>100</v>
-      </c>
-      <c r="J58" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
-      </c>
-      <c r="B59" t="n">
-        <v>0.03689567372202873</v>
-      </c>
-      <c r="C59" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="D59" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="E59" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="F59" t="n">
-        <v>256</v>
-      </c>
-      <c r="G59" t="n">
-        <v>160</v>
-      </c>
-      <c r="H59" t="n">
-        <v>96</v>
-      </c>
-      <c r="I59" t="n">
-        <v>100</v>
-      </c>
-      <c r="J59" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="B60" t="n">
-        <v>0.03647158667445183</v>
-      </c>
-      <c r="C60" t="n">
-        <v>0.003</v>
-      </c>
-      <c r="D60" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="E60" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="F60" t="n">
-        <v>512</v>
-      </c>
-      <c r="G60" t="n">
-        <v>224</v>
-      </c>
-      <c r="H60" t="n">
-        <v>96</v>
-      </c>
-      <c r="I60" t="n">
-        <v>100</v>
-      </c>
-      <c r="J60" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="B61" t="n">
-        <v>0.03625954315066338</v>
-      </c>
-      <c r="C61" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="D61" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="E61" t="n">
-        <v>0.003</v>
-      </c>
-      <c r="F61" t="n">
-        <v>256</v>
-      </c>
-      <c r="G61" t="n">
-        <v>128</v>
-      </c>
-      <c r="H61" t="n">
-        <v>96</v>
-      </c>
-      <c r="I61" t="n">
-        <v>100</v>
-      </c>
-      <c r="J61" t="n">
-        <v>10</v>
+      <c r="H71" t="n">
+        <v>128</v>
+      </c>
+      <c r="I71" t="n">
+        <v>100</v>
+      </c>
+      <c r="J71" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>